<commit_message>
new excel functions overhall
</commit_message>
<xml_diff>
--- a/SampleData.xlsx
+++ b/SampleData.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BI149"/>
+  <dimension ref="A1:BI150"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
@@ -35127,7 +35127,6 @@
           <t>11.56</t>
         </is>
       </c>
-      <c r="AA149" t="inlineStr"/>
       <c r="AB149" t="inlineStr">
         <is>
           <t>7002200</t>
@@ -35138,7 +35137,6 @@
           <t>2200</t>
         </is>
       </c>
-      <c r="AD149" t="inlineStr"/>
       <c r="AE149" t="inlineStr">
         <is>
           <t>20.3</t>
@@ -35290,6 +35288,305 @@
         </is>
       </c>
       <c r="BI149" t="inlineStr">
+        <is>
+          <t>146030596</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>2022-06-14 10:00:32</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>20.1</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>26.5</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>18.9</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>24.6</t>
+        </is>
+      </c>
+      <c r="G150" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="H150" t="inlineStr">
+        <is>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="I150" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="J150" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="K150" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="L150" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M150" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N150" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="O150" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="P150" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="Q150" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="R150" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S150" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="T150" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U150" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V150" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="W150" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
+      </c>
+      <c r="X150" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="Y150" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="Z150" t="inlineStr">
+        <is>
+          <t>11.69</t>
+        </is>
+      </c>
+      <c r="AA150" t="inlineStr"/>
+      <c r="AB150" t="inlineStr">
+        <is>
+          <t>7002200</t>
+        </is>
+      </c>
+      <c r="AC150" t="inlineStr">
+        <is>
+          <t>2200</t>
+        </is>
+      </c>
+      <c r="AD150" t="inlineStr"/>
+      <c r="AE150" t="inlineStr">
+        <is>
+          <t>20.2</t>
+        </is>
+      </c>
+      <c r="AF150" t="inlineStr">
+        <is>
+          <t>26.5</t>
+        </is>
+      </c>
+      <c r="AG150" t="inlineStr">
+        <is>
+          <t>19.0</t>
+        </is>
+      </c>
+      <c r="AH150" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="AI150" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="AJ150" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="AK150" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="AL150" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="AM150" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
+      </c>
+      <c r="AN150" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="AO150" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AP150" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="AQ150" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AR150" t="inlineStr">
+        <is>
+          <t>0.16</t>
+        </is>
+      </c>
+      <c r="AS150" t="inlineStr">
+        <is>
+          <t>0.23</t>
+        </is>
+      </c>
+      <c r="AT150" t="inlineStr">
+        <is>
+          <t>0.45</t>
+        </is>
+      </c>
+      <c r="AU150" t="inlineStr">
+        <is>
+          <t>38.81</t>
+        </is>
+      </c>
+      <c r="AV150" t="inlineStr">
+        <is>
+          <t>3567.76</t>
+        </is>
+      </c>
+      <c r="AW150" t="inlineStr">
+        <is>
+          <t>0.24</t>
+        </is>
+      </c>
+      <c r="AX150" t="inlineStr">
+        <is>
+          <t>22.90</t>
+        </is>
+      </c>
+      <c r="AY150" t="inlineStr">
+        <is>
+          <t>2913.03</t>
+        </is>
+      </c>
+      <c r="AZ150" t="inlineStr">
+        <is>
+          <t>2.00</t>
+        </is>
+      </c>
+      <c r="BA150" t="inlineStr">
+        <is>
+          <t>105.56</t>
+        </is>
+      </c>
+      <c r="BB150" t="inlineStr">
+        <is>
+          <t>10317.49</t>
+        </is>
+      </c>
+      <c r="BC150" t="inlineStr">
+        <is>
+          <t>19.0</t>
+        </is>
+      </c>
+      <c r="BD150" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="BE150" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="BF150" t="inlineStr">
+        <is>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="BG150" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="BH150" t="inlineStr">
+        <is>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="BI150" t="inlineStr">
         <is>
           <t>146030596</t>
         </is>

</xml_diff>

<commit_message>
excel writing improvements (overwriting added)
</commit_message>
<xml_diff>
--- a/SampleData.xlsx
+++ b/SampleData.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BI152"/>
+  <dimension ref="A1:BI155"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
@@ -36018,7 +36018,6 @@
           <t>11.27</t>
         </is>
       </c>
-      <c r="AA152" t="inlineStr"/>
       <c r="AB152" t="inlineStr">
         <is>
           <t>7002200</t>
@@ -36029,7 +36028,6 @@
           <t>2200</t>
         </is>
       </c>
-      <c r="AD152" t="inlineStr"/>
       <c r="AE152" t="inlineStr">
         <is>
           <t>22.0</t>
@@ -36181,6 +36179,899 @@
         </is>
       </c>
       <c r="BI152" t="inlineStr">
+        <is>
+          <t>146030596</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>2022-06-16 08:54:37</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>21.1</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>25.8</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>20.0</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>24.5</t>
+        </is>
+      </c>
+      <c r="G153" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="H153" t="inlineStr">
+        <is>
+          <t>46</t>
+        </is>
+      </c>
+      <c r="I153" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="J153" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="K153" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="L153" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M153" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N153" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="O153" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="P153" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="Q153" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="R153" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S153" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="T153" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U153" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V153" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="W153" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="X153" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="Y153" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="Z153" t="inlineStr">
+        <is>
+          <t>10.28</t>
+        </is>
+      </c>
+      <c r="AB153" t="inlineStr">
+        <is>
+          <t>7002200</t>
+        </is>
+      </c>
+      <c r="AC153" t="inlineStr">
+        <is>
+          <t>2200</t>
+        </is>
+      </c>
+      <c r="AE153" t="inlineStr">
+        <is>
+          <t>21.2</t>
+        </is>
+      </c>
+      <c r="AF153" t="inlineStr">
+        <is>
+          <t>25.8</t>
+        </is>
+      </c>
+      <c r="AG153" t="inlineStr">
+        <is>
+          <t>20.0</t>
+        </is>
+      </c>
+      <c r="AH153" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="AI153" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="AJ153" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="AK153" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="AL153" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="AM153" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="AN153" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="AO153" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AP153" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="AQ153" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AR153" t="inlineStr">
+        <is>
+          <t>0.16</t>
+        </is>
+      </c>
+      <c r="AS153" t="inlineStr">
+        <is>
+          <t>0.15</t>
+        </is>
+      </c>
+      <c r="AT153" t="inlineStr">
+        <is>
+          <t>0.12</t>
+        </is>
+      </c>
+      <c r="AU153" t="inlineStr">
+        <is>
+          <t>33.25</t>
+        </is>
+      </c>
+      <c r="AV153" t="inlineStr">
+        <is>
+          <t>3568.69</t>
+        </is>
+      </c>
+      <c r="AW153" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AX153" t="inlineStr">
+        <is>
+          <t>17.78</t>
+        </is>
+      </c>
+      <c r="AY153" t="inlineStr">
+        <is>
+          <t>2913.03</t>
+        </is>
+      </c>
+      <c r="AZ153" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="BA153" t="inlineStr">
+        <is>
+          <t>87.68</t>
+        </is>
+      </c>
+      <c r="BB153" t="inlineStr">
+        <is>
+          <t>10317.52</t>
+        </is>
+      </c>
+      <c r="BC153" t="inlineStr">
+        <is>
+          <t>19.0</t>
+        </is>
+      </c>
+      <c r="BD153" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="BE153" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="BF153" t="inlineStr">
+        <is>
+          <t>46</t>
+        </is>
+      </c>
+      <c r="BG153" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="BH153" t="inlineStr">
+        <is>
+          <t>46</t>
+        </is>
+      </c>
+      <c r="BI153" t="inlineStr">
+        <is>
+          <t>146030596</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>2022-06-16 08:56:16</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>21.3</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>25.9</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>20.2</t>
+        </is>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="F154" t="inlineStr">
+        <is>
+          <t>24.5</t>
+        </is>
+      </c>
+      <c r="G154" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="H154" t="inlineStr">
+        <is>
+          <t>46</t>
+        </is>
+      </c>
+      <c r="I154" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="J154" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="K154" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="L154" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M154" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N154" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="O154" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="P154" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="Q154" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="R154" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S154" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="T154" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U154" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V154" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="W154" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="X154" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="Y154" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="Z154" t="inlineStr">
+        <is>
+          <t>10.28</t>
+        </is>
+      </c>
+      <c r="AB154" t="inlineStr">
+        <is>
+          <t>7002200</t>
+        </is>
+      </c>
+      <c r="AC154" t="inlineStr">
+        <is>
+          <t>2200</t>
+        </is>
+      </c>
+      <c r="AE154" t="inlineStr">
+        <is>
+          <t>21.4</t>
+        </is>
+      </c>
+      <c r="AF154" t="inlineStr">
+        <is>
+          <t>25.9</t>
+        </is>
+      </c>
+      <c r="AG154" t="inlineStr">
+        <is>
+          <t>20.2</t>
+        </is>
+      </c>
+      <c r="AH154" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="AI154" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="AJ154" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="AK154" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="AL154" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="AM154" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="AN154" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="AO154" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AP154" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="AQ154" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AR154" t="inlineStr">
+        <is>
+          <t>0.16</t>
+        </is>
+      </c>
+      <c r="AS154" t="inlineStr">
+        <is>
+          <t>0.15</t>
+        </is>
+      </c>
+      <c r="AT154" t="inlineStr">
+        <is>
+          <t>0.12</t>
+        </is>
+      </c>
+      <c r="AU154" t="inlineStr">
+        <is>
+          <t>33.25</t>
+        </is>
+      </c>
+      <c r="AV154" t="inlineStr">
+        <is>
+          <t>3568.69</t>
+        </is>
+      </c>
+      <c r="AW154" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AX154" t="inlineStr">
+        <is>
+          <t>17.78</t>
+        </is>
+      </c>
+      <c r="AY154" t="inlineStr">
+        <is>
+          <t>2913.03</t>
+        </is>
+      </c>
+      <c r="AZ154" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="BA154" t="inlineStr">
+        <is>
+          <t>87.68</t>
+        </is>
+      </c>
+      <c r="BB154" t="inlineStr">
+        <is>
+          <t>10317.52</t>
+        </is>
+      </c>
+      <c r="BC154" t="inlineStr">
+        <is>
+          <t>19.0</t>
+        </is>
+      </c>
+      <c r="BD154" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="BE154" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="BF154" t="inlineStr">
+        <is>
+          <t>46</t>
+        </is>
+      </c>
+      <c r="BG154" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="BH154" t="inlineStr">
+        <is>
+          <t>46</t>
+        </is>
+      </c>
+      <c r="BI154" t="inlineStr">
+        <is>
+          <t>146030596</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>2022-06-16 18:19:22</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>23.4</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>26.4</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>22.1</t>
+        </is>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="F155" t="inlineStr">
+        <is>
+          <t>24.9</t>
+        </is>
+      </c>
+      <c r="G155" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="H155" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
+      </c>
+      <c r="I155" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="J155" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="K155" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="L155" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M155" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N155" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="O155" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="P155" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="Q155" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="R155" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S155" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="T155" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U155" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V155" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="W155" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="X155" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="Y155" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="Z155" t="inlineStr">
+        <is>
+          <t>9.84</t>
+        </is>
+      </c>
+      <c r="AA155" t="inlineStr"/>
+      <c r="AB155" t="inlineStr">
+        <is>
+          <t>7002200</t>
+        </is>
+      </c>
+      <c r="AC155" t="inlineStr">
+        <is>
+          <t>2200</t>
+        </is>
+      </c>
+      <c r="AD155" t="inlineStr"/>
+      <c r="AE155" t="inlineStr">
+        <is>
+          <t>23.3</t>
+        </is>
+      </c>
+      <c r="AF155" t="inlineStr">
+        <is>
+          <t>26.4</t>
+        </is>
+      </c>
+      <c r="AG155" t="inlineStr">
+        <is>
+          <t>22.2</t>
+        </is>
+      </c>
+      <c r="AH155" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="AI155" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="AJ155" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="AK155" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="AL155" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="AM155" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="AN155" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="AO155" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AP155" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="AQ155" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AR155" t="inlineStr">
+        <is>
+          <t>0.16</t>
+        </is>
+      </c>
+      <c r="AS155" t="inlineStr">
+        <is>
+          <t>0.16</t>
+        </is>
+      </c>
+      <c r="AT155" t="inlineStr">
+        <is>
+          <t>0.36</t>
+        </is>
+      </c>
+      <c r="AU155" t="inlineStr">
+        <is>
+          <t>33.50</t>
+        </is>
+      </c>
+      <c r="AV155" t="inlineStr">
+        <is>
+          <t>3568.94</t>
+        </is>
+      </c>
+      <c r="AW155" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AX155" t="inlineStr">
+        <is>
+          <t>17.78</t>
+        </is>
+      </c>
+      <c r="AY155" t="inlineStr">
+        <is>
+          <t>2913.03</t>
+        </is>
+      </c>
+      <c r="AZ155" t="inlineStr">
+        <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="BA155" t="inlineStr">
+        <is>
+          <t>87.69</t>
+        </is>
+      </c>
+      <c r="BB155" t="inlineStr">
+        <is>
+          <t>10317.53</t>
+        </is>
+      </c>
+      <c r="BC155" t="inlineStr">
+        <is>
+          <t>19.0</t>
+        </is>
+      </c>
+      <c r="BD155" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="BE155" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="BF155" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
+      </c>
+      <c r="BG155" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="BH155" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
+      </c>
+      <c r="BI155" t="inlineStr">
         <is>
           <t>146030596</t>
         </is>

</xml_diff>

<commit_message>
sample config file added
</commit_message>
<xml_diff>
--- a/SampleData.xlsx
+++ b/SampleData.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BI179"/>
+  <dimension ref="A1:BI180"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
@@ -44037,7 +44037,6 @@
           <t>11.65</t>
         </is>
       </c>
-      <c r="AA179" t="inlineStr"/>
       <c r="AB179" t="inlineStr">
         <is>
           <t>7002200</t>
@@ -44048,7 +44047,6 @@
           <t>2200</t>
         </is>
       </c>
-      <c r="AD179" t="inlineStr"/>
       <c r="AE179" t="inlineStr">
         <is>
           <t>22.2</t>
@@ -44202,6 +44200,305 @@
       <c r="BI179" t="inlineStr">
         <is>
           <t>149177348</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>2022-07-19 17:23:46</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>28.3</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>28.6</t>
+        </is>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>26.7</t>
+        </is>
+      </c>
+      <c r="E180" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="F180" t="inlineStr">
+        <is>
+          <t>25.7</t>
+        </is>
+      </c>
+      <c r="G180" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="H180" t="inlineStr">
+        <is>
+          <t>56</t>
+        </is>
+      </c>
+      <c r="I180" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="J180" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="K180" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="L180" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M180" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N180" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="O180" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="P180" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="Q180" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="R180" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S180" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="T180" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U180" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V180" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="W180" t="inlineStr">
+        <is>
+          <t>69</t>
+        </is>
+      </c>
+      <c r="X180" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="Y180" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="Z180" t="inlineStr">
+        <is>
+          <t>13.40</t>
+        </is>
+      </c>
+      <c r="AA180" t="inlineStr"/>
+      <c r="AB180" t="inlineStr">
+        <is>
+          <t>7002200</t>
+        </is>
+      </c>
+      <c r="AC180" t="inlineStr">
+        <is>
+          <t>2200</t>
+        </is>
+      </c>
+      <c r="AD180" t="inlineStr"/>
+      <c r="AE180" t="inlineStr">
+        <is>
+          <t>28.1</t>
+        </is>
+      </c>
+      <c r="AF180" t="inlineStr">
+        <is>
+          <t>28.6</t>
+        </is>
+      </c>
+      <c r="AG180" t="inlineStr">
+        <is>
+          <t>26.7</t>
+        </is>
+      </c>
+      <c r="AH180" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AI180" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AJ180" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AK180" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="AL180" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="AM180" t="inlineStr">
+        <is>
+          <t>69</t>
+        </is>
+      </c>
+      <c r="AN180" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="AO180" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AP180" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="AQ180" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AR180" t="inlineStr">
+        <is>
+          <t>0.15</t>
+        </is>
+      </c>
+      <c r="AS180" t="inlineStr">
+        <is>
+          <t>0.19</t>
+        </is>
+      </c>
+      <c r="AT180" t="inlineStr">
+        <is>
+          <t>0.29</t>
+        </is>
+      </c>
+      <c r="AU180" t="inlineStr">
+        <is>
+          <t>11.51</t>
+        </is>
+      </c>
+      <c r="AV180" t="inlineStr">
+        <is>
+          <t>3582.14</t>
+        </is>
+      </c>
+      <c r="AW180" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AX180" t="inlineStr">
+        <is>
+          <t>0.14</t>
+        </is>
+      </c>
+      <c r="AY180" t="inlineStr">
+        <is>
+          <t>2913.20</t>
+        </is>
+      </c>
+      <c r="AZ180" t="inlineStr">
+        <is>
+          <t>0.23</t>
+        </is>
+      </c>
+      <c r="BA180" t="inlineStr">
+        <is>
+          <t>8.69</t>
+        </is>
+      </c>
+      <c r="BB180" t="inlineStr">
+        <is>
+          <t>10329.57</t>
+        </is>
+      </c>
+      <c r="BC180" t="inlineStr">
+        <is>
+          <t>19.0</t>
+        </is>
+      </c>
+      <c r="BD180" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="BE180" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="BF180" t="inlineStr">
+        <is>
+          <t>56</t>
+        </is>
+      </c>
+      <c r="BG180" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="BH180" t="inlineStr">
+        <is>
+          <t>56</t>
+        </is>
+      </c>
+      <c r="BI180" t="inlineStr">
+        <is>
+          <t>150225156</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
removed functions that are not supported soon on Selenium
</commit_message>
<xml_diff>
--- a/SampleData.xlsx
+++ b/SampleData.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BI183"/>
+  <dimension ref="A1:BI185"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
@@ -45225,7 +45225,6 @@
           <t>12.81</t>
         </is>
       </c>
-      <c r="AA183" t="inlineStr"/>
       <c r="AB183" t="inlineStr">
         <is>
           <t>7002200</t>
@@ -45236,7 +45235,6 @@
           <t>2200</t>
         </is>
       </c>
-      <c r="AD183" t="inlineStr"/>
       <c r="AE183" t="inlineStr">
         <is>
           <t>22.5</t>
@@ -45390,6 +45388,602 @@
       <c r="BI183" t="inlineStr">
         <is>
           <t>149177348</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>2022-07-26 14:24:35</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>26.6</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>27.2</t>
+        </is>
+      </c>
+      <c r="D184" t="inlineStr">
+        <is>
+          <t>25.8</t>
+        </is>
+      </c>
+      <c r="E184" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="F184" t="inlineStr">
+        <is>
+          <t>25.6</t>
+        </is>
+      </c>
+      <c r="G184" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="H184" t="inlineStr">
+        <is>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="I184" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="J184" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="K184" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="L184" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M184" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N184" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="O184" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="P184" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="Q184" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="R184" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S184" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="T184" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U184" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V184" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="W184" t="inlineStr">
+        <is>
+          <t>72</t>
+        </is>
+      </c>
+      <c r="X184" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="Y184" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="Z184" t="inlineStr">
+        <is>
+          <t>12.61</t>
+        </is>
+      </c>
+      <c r="AB184" t="inlineStr">
+        <is>
+          <t>7002200</t>
+        </is>
+      </c>
+      <c r="AC184" t="inlineStr">
+        <is>
+          <t>2200</t>
+        </is>
+      </c>
+      <c r="AE184" t="inlineStr">
+        <is>
+          <t>26.7</t>
+        </is>
+      </c>
+      <c r="AF184" t="inlineStr">
+        <is>
+          <t>27.3</t>
+        </is>
+      </c>
+      <c r="AG184" t="inlineStr">
+        <is>
+          <t>25.7</t>
+        </is>
+      </c>
+      <c r="AH184" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AI184" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AJ184" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AK184" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="AL184" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="AM184" t="inlineStr">
+        <is>
+          <t>72</t>
+        </is>
+      </c>
+      <c r="AN184" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="AO184" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AP184" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="AQ184" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AR184" t="inlineStr">
+        <is>
+          <t>0.15</t>
+        </is>
+      </c>
+      <c r="AS184" t="inlineStr">
+        <is>
+          <t>0.16</t>
+        </is>
+      </c>
+      <c r="AT184" t="inlineStr">
+        <is>
+          <t>0.21</t>
+        </is>
+      </c>
+      <c r="AU184" t="inlineStr">
+        <is>
+          <t>11.23</t>
+        </is>
+      </c>
+      <c r="AV184" t="inlineStr">
+        <is>
+          <t>3584.69</t>
+        </is>
+      </c>
+      <c r="AW184" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AX184" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AY184" t="inlineStr">
+        <is>
+          <t>2913.20</t>
+        </is>
+      </c>
+      <c r="AZ184" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="BA184" t="inlineStr">
+        <is>
+          <t>4.68</t>
+        </is>
+      </c>
+      <c r="BB184" t="inlineStr">
+        <is>
+          <t>10331.15</t>
+        </is>
+      </c>
+      <c r="BC184" t="inlineStr">
+        <is>
+          <t>19.0</t>
+        </is>
+      </c>
+      <c r="BD184" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="BE184" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="BF184" t="inlineStr">
+        <is>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="BG184" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="BH184" t="inlineStr">
+        <is>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="BI184" t="inlineStr">
+        <is>
+          <t>149176580</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>2022-07-26 14:24:49</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>26.6</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>27.1</t>
+        </is>
+      </c>
+      <c r="D185" t="inlineStr">
+        <is>
+          <t>25.7</t>
+        </is>
+      </c>
+      <c r="E185" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="F185" t="inlineStr">
+        <is>
+          <t>25.6</t>
+        </is>
+      </c>
+      <c r="G185" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="H185" t="inlineStr">
+        <is>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="I185" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="J185" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="K185" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="L185" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M185" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N185" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="O185" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="P185" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="Q185" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="R185" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S185" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="T185" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U185" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V185" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="W185" t="inlineStr">
+        <is>
+          <t>72</t>
+        </is>
+      </c>
+      <c r="X185" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="Y185" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="Z185" t="inlineStr">
+        <is>
+          <t>12.61</t>
+        </is>
+      </c>
+      <c r="AA185" t="inlineStr"/>
+      <c r="AB185" t="inlineStr">
+        <is>
+          <t>7002200</t>
+        </is>
+      </c>
+      <c r="AC185" t="inlineStr">
+        <is>
+          <t>2200</t>
+        </is>
+      </c>
+      <c r="AD185" t="inlineStr"/>
+      <c r="AE185" t="inlineStr">
+        <is>
+          <t>26.5</t>
+        </is>
+      </c>
+      <c r="AF185" t="inlineStr">
+        <is>
+          <t>27.2</t>
+        </is>
+      </c>
+      <c r="AG185" t="inlineStr">
+        <is>
+          <t>25.7</t>
+        </is>
+      </c>
+      <c r="AH185" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AI185" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AJ185" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AK185" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="AL185" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="AM185" t="inlineStr">
+        <is>
+          <t>72</t>
+        </is>
+      </c>
+      <c r="AN185" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="AO185" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AP185" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="AQ185" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AR185" t="inlineStr">
+        <is>
+          <t>0.15</t>
+        </is>
+      </c>
+      <c r="AS185" t="inlineStr">
+        <is>
+          <t>0.16</t>
+        </is>
+      </c>
+      <c r="AT185" t="inlineStr">
+        <is>
+          <t>0.21</t>
+        </is>
+      </c>
+      <c r="AU185" t="inlineStr">
+        <is>
+          <t>11.23</t>
+        </is>
+      </c>
+      <c r="AV185" t="inlineStr">
+        <is>
+          <t>3584.69</t>
+        </is>
+      </c>
+      <c r="AW185" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AX185" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AY185" t="inlineStr">
+        <is>
+          <t>2913.20</t>
+        </is>
+      </c>
+      <c r="AZ185" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="BA185" t="inlineStr">
+        <is>
+          <t>4.68</t>
+        </is>
+      </c>
+      <c r="BB185" t="inlineStr">
+        <is>
+          <t>10331.15</t>
+        </is>
+      </c>
+      <c r="BC185" t="inlineStr">
+        <is>
+          <t>19.0</t>
+        </is>
+      </c>
+      <c r="BD185" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="BE185" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="BF185" t="inlineStr">
+        <is>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="BG185" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="BH185" t="inlineStr">
+        <is>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="BI185" t="inlineStr">
+        <is>
+          <t>149176580</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Functions input formatting more readable
</commit_message>
<xml_diff>
--- a/SampleData.xlsx
+++ b/SampleData.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BI185"/>
+  <dimension ref="A1:BI186"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
@@ -45819,7 +45819,6 @@
           <t>12.61</t>
         </is>
       </c>
-      <c r="AA185" t="inlineStr"/>
       <c r="AB185" t="inlineStr">
         <is>
           <t>7002200</t>
@@ -45830,7 +45829,6 @@
           <t>2200</t>
         </is>
       </c>
-      <c r="AD185" t="inlineStr"/>
       <c r="AE185" t="inlineStr">
         <is>
           <t>26.5</t>
@@ -45984,6 +45982,305 @@
       <c r="BI185" t="inlineStr">
         <is>
           <t>149176580</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>2022-07-27 12:43:00</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>23.9</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>26.3</t>
+        </is>
+      </c>
+      <c r="D186" t="inlineStr">
+        <is>
+          <t>22.9</t>
+        </is>
+      </c>
+      <c r="E186" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="F186" t="inlineStr">
+        <is>
+          <t>24.9</t>
+        </is>
+      </c>
+      <c r="G186" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="H186" t="inlineStr">
+        <is>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="I186" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="J186" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="K186" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="L186" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M186" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N186" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="O186" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="P186" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="Q186" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="R186" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S186" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="T186" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U186" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V186" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="W186" t="inlineStr">
+        <is>
+          <t>73</t>
+        </is>
+      </c>
+      <c r="X186" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="Y186" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="Z186" t="inlineStr">
+        <is>
+          <t>11.89</t>
+        </is>
+      </c>
+      <c r="AA186" t="inlineStr"/>
+      <c r="AB186" t="inlineStr">
+        <is>
+          <t>7002200</t>
+        </is>
+      </c>
+      <c r="AC186" t="inlineStr">
+        <is>
+          <t>2200</t>
+        </is>
+      </c>
+      <c r="AD186" t="inlineStr"/>
+      <c r="AE186" t="inlineStr">
+        <is>
+          <t>24.0</t>
+        </is>
+      </c>
+      <c r="AF186" t="inlineStr">
+        <is>
+          <t>26.3</t>
+        </is>
+      </c>
+      <c r="AG186" t="inlineStr">
+        <is>
+          <t>22.8</t>
+        </is>
+      </c>
+      <c r="AH186" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="AI186" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="AJ186" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="AK186" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="AL186" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="AM186" t="inlineStr">
+        <is>
+          <t>73</t>
+        </is>
+      </c>
+      <c r="AN186" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="AO186" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AP186" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="AQ186" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AR186" t="inlineStr">
+        <is>
+          <t>0.17</t>
+        </is>
+      </c>
+      <c r="AS186" t="inlineStr">
+        <is>
+          <t>0.16</t>
+        </is>
+      </c>
+      <c r="AT186" t="inlineStr">
+        <is>
+          <t>0.23</t>
+        </is>
+      </c>
+      <c r="AU186" t="inlineStr">
+        <is>
+          <t>11.24</t>
+        </is>
+      </c>
+      <c r="AV186" t="inlineStr">
+        <is>
+          <t>3585.03</t>
+        </is>
+      </c>
+      <c r="AW186" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AX186" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AY186" t="inlineStr">
+        <is>
+          <t>2913.20</t>
+        </is>
+      </c>
+      <c r="AZ186" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="BA186" t="inlineStr">
+        <is>
+          <t>4.16</t>
+        </is>
+      </c>
+      <c r="BB186" t="inlineStr">
+        <is>
+          <t>10331.16</t>
+        </is>
+      </c>
+      <c r="BC186" t="inlineStr">
+        <is>
+          <t>19.0</t>
+        </is>
+      </c>
+      <c r="BD186" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="BE186" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="BF186" t="inlineStr">
+        <is>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="BG186" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="BH186" t="inlineStr">
+        <is>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="BI186" t="inlineStr">
+        <is>
+          <t>150225924</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Yahoo finance lib return change if compare changed
</commit_message>
<xml_diff>
--- a/SampleData.xlsx
+++ b/SampleData.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BI303"/>
+  <dimension ref="A1:BI306"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
@@ -80865,7 +80865,6 @@
           <t>12.68</t>
         </is>
       </c>
-      <c r="AA303" t="inlineStr"/>
       <c r="AB303" t="inlineStr">
         <is>
           <t>000000</t>
@@ -80876,7 +80875,6 @@
           <t>000</t>
         </is>
       </c>
-      <c r="AD303" t="inlineStr"/>
       <c r="AE303" t="inlineStr">
         <is>
           <t>24.1</t>
@@ -81028,6 +81026,899 @@
         </is>
       </c>
       <c r="BI303" t="inlineStr">
+        <is>
+          <t>140649476</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>2023-07-12 10:45:00</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>25.2</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>26.7</t>
+        </is>
+      </c>
+      <c r="D304" t="inlineStr">
+        <is>
+          <t>23.7</t>
+        </is>
+      </c>
+      <c r="E304" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="F304" t="inlineStr">
+        <is>
+          <t>24.2</t>
+        </is>
+      </c>
+      <c r="G304" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="H304" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
+      </c>
+      <c r="I304" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="J304" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="K304" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="L304" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="M304" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N304" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="O304" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="P304" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="Q304" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="R304" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S304" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="T304" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U304" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V304" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="W304" t="inlineStr">
+        <is>
+          <t>74</t>
+        </is>
+      </c>
+      <c r="X304" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="Y304" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="Z304" t="inlineStr">
+        <is>
+          <t>9.46</t>
+        </is>
+      </c>
+      <c r="AB304" t="inlineStr">
+        <is>
+          <t>000000</t>
+        </is>
+      </c>
+      <c r="AC304" t="inlineStr">
+        <is>
+          <t>000</t>
+        </is>
+      </c>
+      <c r="AE304" t="inlineStr">
+        <is>
+          <t>25.1</t>
+        </is>
+      </c>
+      <c r="AF304" t="inlineStr">
+        <is>
+          <t>26.7</t>
+        </is>
+      </c>
+      <c r="AG304" t="inlineStr">
+        <is>
+          <t>23.8</t>
+        </is>
+      </c>
+      <c r="AH304" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AI304" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AJ304" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AK304" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AL304" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AM304" t="inlineStr">
+        <is>
+          <t>74</t>
+        </is>
+      </c>
+      <c r="AN304" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="AO304" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AP304" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="AQ304" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AR304" t="inlineStr">
+        <is>
+          <t>0.15</t>
+        </is>
+      </c>
+      <c r="AS304" t="inlineStr">
+        <is>
+          <t>0.15</t>
+        </is>
+      </c>
+      <c r="AT304" t="inlineStr">
+        <is>
+          <t>0.10</t>
+        </is>
+      </c>
+      <c r="AU304" t="inlineStr">
+        <is>
+          <t>8.00</t>
+        </is>
+      </c>
+      <c r="AV304" t="inlineStr">
+        <is>
+          <t>4473.60</t>
+        </is>
+      </c>
+      <c r="AW304" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AX304" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AY304" t="inlineStr">
+        <is>
+          <t>3634.20</t>
+        </is>
+      </c>
+      <c r="AZ304" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="BA304" t="inlineStr">
+        <is>
+          <t>5.55</t>
+        </is>
+      </c>
+      <c r="BB304" t="inlineStr">
+        <is>
+          <t>12870.25</t>
+        </is>
+      </c>
+      <c r="BC304" t="inlineStr">
+        <is>
+          <t>19.0</t>
+        </is>
+      </c>
+      <c r="BD304" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="BE304" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="BF304" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
+      </c>
+      <c r="BG304" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="BH304" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
+      </c>
+      <c r="BI304" t="inlineStr">
+        <is>
+          <t>140649476</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>2023-07-13 12:41:36</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>27.5</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>26.7</t>
+        </is>
+      </c>
+      <c r="D305" t="inlineStr">
+        <is>
+          <t>25.9</t>
+        </is>
+      </c>
+      <c r="E305" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="F305" t="inlineStr">
+        <is>
+          <t>24.9</t>
+        </is>
+      </c>
+      <c r="G305" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="H305" t="inlineStr">
+        <is>
+          <t>38</t>
+        </is>
+      </c>
+      <c r="I305" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="J305" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="K305" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="L305" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M305" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N305" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="O305" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="P305" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="Q305" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="R305" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S305" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="T305" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U305" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V305" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="W305" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="X305" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="Y305" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="Z305" t="inlineStr">
+        <is>
+          <t>8.69</t>
+        </is>
+      </c>
+      <c r="AB305" t="inlineStr">
+        <is>
+          <t>000000</t>
+        </is>
+      </c>
+      <c r="AC305" t="inlineStr">
+        <is>
+          <t>000</t>
+        </is>
+      </c>
+      <c r="AE305" t="inlineStr">
+        <is>
+          <t>27.3</t>
+        </is>
+      </c>
+      <c r="AF305" t="inlineStr">
+        <is>
+          <t>26.9</t>
+        </is>
+      </c>
+      <c r="AG305" t="inlineStr">
+        <is>
+          <t>26.1</t>
+        </is>
+      </c>
+      <c r="AH305" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AI305" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AJ305" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AK305" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AL305" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AM305" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="AN305" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="AO305" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AP305" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="AQ305" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AR305" t="inlineStr">
+        <is>
+          <t>0.15</t>
+        </is>
+      </c>
+      <c r="AS305" t="inlineStr">
+        <is>
+          <t>0.15</t>
+        </is>
+      </c>
+      <c r="AT305" t="inlineStr">
+        <is>
+          <t>0.11</t>
+        </is>
+      </c>
+      <c r="AU305" t="inlineStr">
+        <is>
+          <t>8.03</t>
+        </is>
+      </c>
+      <c r="AV305" t="inlineStr">
+        <is>
+          <t>4473.90</t>
+        </is>
+      </c>
+      <c r="AW305" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AX305" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AY305" t="inlineStr">
+        <is>
+          <t>3634.20</t>
+        </is>
+      </c>
+      <c r="AZ305" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="BA305" t="inlineStr">
+        <is>
+          <t>5.51</t>
+        </is>
+      </c>
+      <c r="BB305" t="inlineStr">
+        <is>
+          <t>12870.46</t>
+        </is>
+      </c>
+      <c r="BC305" t="inlineStr">
+        <is>
+          <t>19.0</t>
+        </is>
+      </c>
+      <c r="BD305" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="BE305" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="BF305" t="inlineStr">
+        <is>
+          <t>38</t>
+        </is>
+      </c>
+      <c r="BG305" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="BH305" t="inlineStr">
+        <is>
+          <t>38</t>
+        </is>
+      </c>
+      <c r="BI305" t="inlineStr">
+        <is>
+          <t>140648452</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>2023-07-14 10:23:56</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>24.8</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>26.9</t>
+        </is>
+      </c>
+      <c r="D306" t="inlineStr">
+        <is>
+          <t>21.5</t>
+        </is>
+      </c>
+      <c r="E306" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="F306" t="inlineStr">
+        <is>
+          <t>24.4</t>
+        </is>
+      </c>
+      <c r="G306" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="H306" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="I306" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="J306" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="K306" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="L306" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M306" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N306" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="O306" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="P306" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="Q306" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="R306" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S306" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="T306" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U306" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V306" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="W306" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="X306" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="Y306" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="Z306" t="inlineStr">
+        <is>
+          <t>12.01</t>
+        </is>
+      </c>
+      <c r="AA306" t="inlineStr"/>
+      <c r="AB306" t="inlineStr">
+        <is>
+          <t>000000</t>
+        </is>
+      </c>
+      <c r="AC306" t="inlineStr">
+        <is>
+          <t>000</t>
+        </is>
+      </c>
+      <c r="AD306" t="inlineStr"/>
+      <c r="AE306" t="inlineStr">
+        <is>
+          <t>24.7</t>
+        </is>
+      </c>
+      <c r="AF306" t="inlineStr">
+        <is>
+          <t>26.9</t>
+        </is>
+      </c>
+      <c r="AG306" t="inlineStr">
+        <is>
+          <t>21.6</t>
+        </is>
+      </c>
+      <c r="AH306" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AI306" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AJ306" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AK306" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AL306" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AM306" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="AN306" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="AO306" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AP306" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="AQ306" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AR306" t="inlineStr">
+        <is>
+          <t>0.15</t>
+        </is>
+      </c>
+      <c r="AS306" t="inlineStr">
+        <is>
+          <t>0.15</t>
+        </is>
+      </c>
+      <c r="AT306" t="inlineStr">
+        <is>
+          <t>0.09</t>
+        </is>
+      </c>
+      <c r="AU306" t="inlineStr">
+        <is>
+          <t>7.97</t>
+        </is>
+      </c>
+      <c r="AV306" t="inlineStr">
+        <is>
+          <t>4474.13</t>
+        </is>
+      </c>
+      <c r="AW306" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AX306" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AY306" t="inlineStr">
+        <is>
+          <t>3634.20</t>
+        </is>
+      </c>
+      <c r="AZ306" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="BA306" t="inlineStr">
+        <is>
+          <t>5.25</t>
+        </is>
+      </c>
+      <c r="BB306" t="inlineStr">
+        <is>
+          <t>12870.46</t>
+        </is>
+      </c>
+      <c r="BC306" t="inlineStr">
+        <is>
+          <t>19.0</t>
+        </is>
+      </c>
+      <c r="BD306" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="BE306" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="BF306" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="BG306" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="BH306" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="BI306" t="inlineStr">
         <is>
           <t>140649476</t>
         </is>

</xml_diff>

<commit_message>
Chrome driver code consolidated to one place
</commit_message>
<xml_diff>
--- a/SampleData.xlsx
+++ b/SampleData.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BI307"/>
+  <dimension ref="A1:BI313"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
@@ -82053,7 +82053,6 @@
           <t>11.50</t>
         </is>
       </c>
-      <c r="AA307" t="inlineStr"/>
       <c r="AB307" t="inlineStr">
         <is>
           <t>000000</t>
@@ -82064,7 +82063,6 @@
           <t>000</t>
         </is>
       </c>
-      <c r="AD307" t="inlineStr"/>
       <c r="AE307" t="inlineStr">
         <is>
           <t>26.6</t>
@@ -82218,6 +82216,1790 @@
       <c r="BI307" t="inlineStr">
         <is>
           <t>140648452</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>2023-07-19 19:43:21</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>26.0</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>27.8</t>
+        </is>
+      </c>
+      <c r="D308" t="inlineStr">
+        <is>
+          <t>22.5</t>
+        </is>
+      </c>
+      <c r="E308" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="F308" t="inlineStr">
+        <is>
+          <t>24.5</t>
+        </is>
+      </c>
+      <c r="G308" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="H308" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
+      </c>
+      <c r="I308" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="J308" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="K308" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="L308" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M308" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N308" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="O308" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="P308" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="Q308" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="R308" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S308" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="T308" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U308" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V308" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="W308" t="inlineStr">
+        <is>
+          <t>78</t>
+        </is>
+      </c>
+      <c r="X308" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="Y308" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="Z308" t="inlineStr">
+        <is>
+          <t>10.73</t>
+        </is>
+      </c>
+      <c r="AB308" t="inlineStr">
+        <is>
+          <t>000000</t>
+        </is>
+      </c>
+      <c r="AC308" t="inlineStr">
+        <is>
+          <t>000</t>
+        </is>
+      </c>
+      <c r="AE308" t="inlineStr">
+        <is>
+          <t>26.0</t>
+        </is>
+      </c>
+      <c r="AF308" t="inlineStr">
+        <is>
+          <t>27.7</t>
+        </is>
+      </c>
+      <c r="AG308" t="inlineStr">
+        <is>
+          <t>22.6</t>
+        </is>
+      </c>
+      <c r="AH308" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AI308" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AJ308" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AK308" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AL308" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AM308" t="inlineStr">
+        <is>
+          <t>78</t>
+        </is>
+      </c>
+      <c r="AN308" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="AO308" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AP308" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="AQ308" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AR308" t="inlineStr">
+        <is>
+          <t>0.15</t>
+        </is>
+      </c>
+      <c r="AS308" t="inlineStr">
+        <is>
+          <t>0.17</t>
+        </is>
+      </c>
+      <c r="AT308" t="inlineStr">
+        <is>
+          <t>0.21</t>
+        </is>
+      </c>
+      <c r="AU308" t="inlineStr">
+        <is>
+          <t>7.97</t>
+        </is>
+      </c>
+      <c r="AV308" t="inlineStr">
+        <is>
+          <t>4475.60</t>
+        </is>
+      </c>
+      <c r="AW308" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AX308" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AY308" t="inlineStr">
+        <is>
+          <t>3634.20</t>
+        </is>
+      </c>
+      <c r="AZ308" t="inlineStr">
+        <is>
+          <t>0.10</t>
+        </is>
+      </c>
+      <c r="BA308" t="inlineStr">
+        <is>
+          <t>4.02</t>
+        </is>
+      </c>
+      <c r="BB308" t="inlineStr">
+        <is>
+          <t>12871.02</t>
+        </is>
+      </c>
+      <c r="BC308" t="inlineStr">
+        <is>
+          <t>19.0</t>
+        </is>
+      </c>
+      <c r="BD308" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="BE308" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="BF308" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
+      </c>
+      <c r="BG308" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="BH308" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
+      </c>
+      <c r="BI308" t="inlineStr">
+        <is>
+          <t>140649476</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>2023-07-22 19:48:07</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>23.9</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>26.9</t>
+        </is>
+      </c>
+      <c r="D309" t="inlineStr">
+        <is>
+          <t>18.9</t>
+        </is>
+      </c>
+      <c r="E309" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="F309" t="inlineStr">
+        <is>
+          <t>24.1</t>
+        </is>
+      </c>
+      <c r="G309" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="H309" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="I309" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="J309" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="K309" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="L309" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M309" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="N309" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="O309" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="P309" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="Q309" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="R309" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S309" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="T309" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U309" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V309" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="W309" t="inlineStr">
+        <is>
+          <t>79</t>
+        </is>
+      </c>
+      <c r="X309" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="Y309" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="Z309" t="inlineStr">
+        <is>
+          <t>11.81</t>
+        </is>
+      </c>
+      <c r="AB309" t="inlineStr">
+        <is>
+          <t>000000</t>
+        </is>
+      </c>
+      <c r="AC309" t="inlineStr">
+        <is>
+          <t>000</t>
+        </is>
+      </c>
+      <c r="AE309" t="inlineStr">
+        <is>
+          <t>23.9</t>
+        </is>
+      </c>
+      <c r="AF309" t="inlineStr">
+        <is>
+          <t>27.1</t>
+        </is>
+      </c>
+      <c r="AG309" t="inlineStr">
+        <is>
+          <t>18.9</t>
+        </is>
+      </c>
+      <c r="AH309" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AI309" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AJ309" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AK309" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AL309" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AM309" t="inlineStr">
+        <is>
+          <t>79</t>
+        </is>
+      </c>
+      <c r="AN309" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="AO309" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AP309" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="AQ309" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AR309" t="inlineStr">
+        <is>
+          <t>0.15</t>
+        </is>
+      </c>
+      <c r="AS309" t="inlineStr">
+        <is>
+          <t>0.15</t>
+        </is>
+      </c>
+      <c r="AT309" t="inlineStr">
+        <is>
+          <t>0.19</t>
+        </is>
+      </c>
+      <c r="AU309" t="inlineStr">
+        <is>
+          <t>7.87</t>
+        </is>
+      </c>
+      <c r="AV309" t="inlineStr">
+        <is>
+          <t>4476.34</t>
+        </is>
+      </c>
+      <c r="AW309" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AX309" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AY309" t="inlineStr">
+        <is>
+          <t>3634.20</t>
+        </is>
+      </c>
+      <c r="AZ309" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="BA309" t="inlineStr">
+        <is>
+          <t>3.12</t>
+        </is>
+      </c>
+      <c r="BB309" t="inlineStr">
+        <is>
+          <t>12871.04</t>
+        </is>
+      </c>
+      <c r="BC309" t="inlineStr">
+        <is>
+          <t>19.0</t>
+        </is>
+      </c>
+      <c r="BD309" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="BE309" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="BF309" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="BG309" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="BH309" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="BI309" t="inlineStr">
+        <is>
+          <t>140649476</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>2023-07-22 19:48:50</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>23.8</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>27.0</t>
+        </is>
+      </c>
+      <c r="D310" t="inlineStr">
+        <is>
+          <t>18.9</t>
+        </is>
+      </c>
+      <c r="E310" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="F310" t="inlineStr">
+        <is>
+          <t>24.1</t>
+        </is>
+      </c>
+      <c r="G310" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="H310" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="I310" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="J310" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="K310" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="L310" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M310" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N310" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="O310" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="P310" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="Q310" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="R310" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S310" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="T310" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U310" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V310" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="W310" t="inlineStr">
+        <is>
+          <t>79</t>
+        </is>
+      </c>
+      <c r="X310" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="Y310" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="Z310" t="inlineStr">
+        <is>
+          <t>11.81</t>
+        </is>
+      </c>
+      <c r="AB310" t="inlineStr">
+        <is>
+          <t>000000</t>
+        </is>
+      </c>
+      <c r="AC310" t="inlineStr">
+        <is>
+          <t>000</t>
+        </is>
+      </c>
+      <c r="AE310" t="inlineStr">
+        <is>
+          <t>23.7</t>
+        </is>
+      </c>
+      <c r="AF310" t="inlineStr">
+        <is>
+          <t>27.0</t>
+        </is>
+      </c>
+      <c r="AG310" t="inlineStr">
+        <is>
+          <t>19.0</t>
+        </is>
+      </c>
+      <c r="AH310" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AI310" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AJ310" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AK310" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AL310" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AM310" t="inlineStr">
+        <is>
+          <t>79</t>
+        </is>
+      </c>
+      <c r="AN310" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="AO310" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AP310" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="AQ310" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AR310" t="inlineStr">
+        <is>
+          <t>0.15</t>
+        </is>
+      </c>
+      <c r="AS310" t="inlineStr">
+        <is>
+          <t>0.15</t>
+        </is>
+      </c>
+      <c r="AT310" t="inlineStr">
+        <is>
+          <t>0.19</t>
+        </is>
+      </c>
+      <c r="AU310" t="inlineStr">
+        <is>
+          <t>7.87</t>
+        </is>
+      </c>
+      <c r="AV310" t="inlineStr">
+        <is>
+          <t>4476.34</t>
+        </is>
+      </c>
+      <c r="AW310" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AX310" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AY310" t="inlineStr">
+        <is>
+          <t>3634.20</t>
+        </is>
+      </c>
+      <c r="AZ310" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="BA310" t="inlineStr">
+        <is>
+          <t>3.12</t>
+        </is>
+      </c>
+      <c r="BB310" t="inlineStr">
+        <is>
+          <t>12871.04</t>
+        </is>
+      </c>
+      <c r="BC310" t="inlineStr">
+        <is>
+          <t>19.0</t>
+        </is>
+      </c>
+      <c r="BD310" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="BE310" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="BF310" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="BG310" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="BH310" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="BI310" t="inlineStr">
+        <is>
+          <t>140649476</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>2023-07-22 19:49:12</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>23.8</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>27.2</t>
+        </is>
+      </c>
+      <c r="D311" t="inlineStr">
+        <is>
+          <t>18.9</t>
+        </is>
+      </c>
+      <c r="E311" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="F311" t="inlineStr">
+        <is>
+          <t>24.1</t>
+        </is>
+      </c>
+      <c r="G311" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="H311" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="I311" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="J311" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="K311" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="L311" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M311" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N311" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="O311" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="P311" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="Q311" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="R311" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S311" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="T311" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U311" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V311" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="W311" t="inlineStr">
+        <is>
+          <t>79</t>
+        </is>
+      </c>
+      <c r="X311" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="Y311" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="Z311" t="inlineStr">
+        <is>
+          <t>11.81</t>
+        </is>
+      </c>
+      <c r="AB311" t="inlineStr">
+        <is>
+          <t>000000</t>
+        </is>
+      </c>
+      <c r="AC311" t="inlineStr">
+        <is>
+          <t>000</t>
+        </is>
+      </c>
+      <c r="AE311" t="inlineStr">
+        <is>
+          <t>23.8</t>
+        </is>
+      </c>
+      <c r="AF311" t="inlineStr">
+        <is>
+          <t>27.2</t>
+        </is>
+      </c>
+      <c r="AG311" t="inlineStr">
+        <is>
+          <t>18.8</t>
+        </is>
+      </c>
+      <c r="AH311" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AI311" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AJ311" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AK311" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AL311" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AM311" t="inlineStr">
+        <is>
+          <t>79</t>
+        </is>
+      </c>
+      <c r="AN311" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="AO311" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AP311" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="AQ311" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AR311" t="inlineStr">
+        <is>
+          <t>0.15</t>
+        </is>
+      </c>
+      <c r="AS311" t="inlineStr">
+        <is>
+          <t>0.15</t>
+        </is>
+      </c>
+      <c r="AT311" t="inlineStr">
+        <is>
+          <t>0.19</t>
+        </is>
+      </c>
+      <c r="AU311" t="inlineStr">
+        <is>
+          <t>7.87</t>
+        </is>
+      </c>
+      <c r="AV311" t="inlineStr">
+        <is>
+          <t>4476.34</t>
+        </is>
+      </c>
+      <c r="AW311" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AX311" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AY311" t="inlineStr">
+        <is>
+          <t>3634.20</t>
+        </is>
+      </c>
+      <c r="AZ311" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="BA311" t="inlineStr">
+        <is>
+          <t>3.12</t>
+        </is>
+      </c>
+      <c r="BB311" t="inlineStr">
+        <is>
+          <t>12871.04</t>
+        </is>
+      </c>
+      <c r="BC311" t="inlineStr">
+        <is>
+          <t>19.0</t>
+        </is>
+      </c>
+      <c r="BD311" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="BE311" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="BF311" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="BG311" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="BH311" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="BI311" t="inlineStr">
+        <is>
+          <t>140649476</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>2023-07-23 10:28:08</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>23.8</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>26.0</t>
+        </is>
+      </c>
+      <c r="D312" t="inlineStr">
+        <is>
+          <t>21.0</t>
+        </is>
+      </c>
+      <c r="E312" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="F312" t="inlineStr">
+        <is>
+          <t>23.8</t>
+        </is>
+      </c>
+      <c r="G312" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="H312" t="inlineStr">
+        <is>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="I312" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="J312" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="K312" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="L312" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M312" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N312" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="O312" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="P312" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="Q312" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="R312" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S312" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="T312" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U312" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V312" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="W312" t="inlineStr">
+        <is>
+          <t>79</t>
+        </is>
+      </c>
+      <c r="X312" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="Y312" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="Z312" t="inlineStr">
+        <is>
+          <t>11.18</t>
+        </is>
+      </c>
+      <c r="AB312" t="inlineStr">
+        <is>
+          <t>000000</t>
+        </is>
+      </c>
+      <c r="AC312" t="inlineStr">
+        <is>
+          <t>000</t>
+        </is>
+      </c>
+      <c r="AE312" t="inlineStr">
+        <is>
+          <t>23.9</t>
+        </is>
+      </c>
+      <c r="AF312" t="inlineStr">
+        <is>
+          <t>26.0</t>
+        </is>
+      </c>
+      <c r="AG312" t="inlineStr">
+        <is>
+          <t>20.9</t>
+        </is>
+      </c>
+      <c r="AH312" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AI312" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AJ312" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AK312" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AL312" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AM312" t="inlineStr">
+        <is>
+          <t>79</t>
+        </is>
+      </c>
+      <c r="AN312" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="AO312" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AP312" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="AQ312" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AR312" t="inlineStr">
+        <is>
+          <t>0.15</t>
+        </is>
+      </c>
+      <c r="AS312" t="inlineStr">
+        <is>
+          <t>0.15</t>
+        </is>
+      </c>
+      <c r="AT312" t="inlineStr">
+        <is>
+          <t>0.09</t>
+        </is>
+      </c>
+      <c r="AU312" t="inlineStr">
+        <is>
+          <t>7.74</t>
+        </is>
+      </c>
+      <c r="AV312" t="inlineStr">
+        <is>
+          <t>4476.50</t>
+        </is>
+      </c>
+      <c r="AW312" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AX312" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AY312" t="inlineStr">
+        <is>
+          <t>3634.20</t>
+        </is>
+      </c>
+      <c r="AZ312" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="BA312" t="inlineStr">
+        <is>
+          <t>2.77</t>
+        </is>
+      </c>
+      <c r="BB312" t="inlineStr">
+        <is>
+          <t>12871.04</t>
+        </is>
+      </c>
+      <c r="BC312" t="inlineStr">
+        <is>
+          <t>19.0</t>
+        </is>
+      </c>
+      <c r="BD312" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="BE312" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="BF312" t="inlineStr">
+        <is>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="BG312" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="BH312" t="inlineStr">
+        <is>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="BI312" t="inlineStr">
+        <is>
+          <t>140649476</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>2023-07-23 10:42:05</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>23.9</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>26.3</t>
+        </is>
+      </c>
+      <c r="D313" t="inlineStr">
+        <is>
+          <t>21.0</t>
+        </is>
+      </c>
+      <c r="E313" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="F313" t="inlineStr">
+        <is>
+          <t>23.8</t>
+        </is>
+      </c>
+      <c r="G313" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="H313" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="I313" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="J313" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="K313" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="L313" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M313" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N313" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="O313" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="P313" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="Q313" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="R313" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S313" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="T313" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U313" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V313" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="W313" t="inlineStr">
+        <is>
+          <t>79</t>
+        </is>
+      </c>
+      <c r="X313" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="Y313" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="Z313" t="inlineStr">
+        <is>
+          <t>10.97</t>
+        </is>
+      </c>
+      <c r="AA313" t="inlineStr"/>
+      <c r="AB313" t="inlineStr">
+        <is>
+          <t>000000</t>
+        </is>
+      </c>
+      <c r="AC313" t="inlineStr">
+        <is>
+          <t>000</t>
+        </is>
+      </c>
+      <c r="AD313" t="inlineStr"/>
+      <c r="AE313" t="inlineStr">
+        <is>
+          <t>24.0</t>
+        </is>
+      </c>
+      <c r="AF313" t="inlineStr">
+        <is>
+          <t>26.2</t>
+        </is>
+      </c>
+      <c r="AG313" t="inlineStr">
+        <is>
+          <t>20.8</t>
+        </is>
+      </c>
+      <c r="AH313" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AI313" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AJ313" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AK313" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AL313" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AM313" t="inlineStr">
+        <is>
+          <t>79</t>
+        </is>
+      </c>
+      <c r="AN313" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="AO313" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AP313" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="AQ313" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AR313" t="inlineStr">
+        <is>
+          <t>0.15</t>
+        </is>
+      </c>
+      <c r="AS313" t="inlineStr">
+        <is>
+          <t>0.15</t>
+        </is>
+      </c>
+      <c r="AT313" t="inlineStr">
+        <is>
+          <t>0.10</t>
+        </is>
+      </c>
+      <c r="AU313" t="inlineStr">
+        <is>
+          <t>7.74</t>
+        </is>
+      </c>
+      <c r="AV313" t="inlineStr">
+        <is>
+          <t>4476.50</t>
+        </is>
+      </c>
+      <c r="AW313" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AX313" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AY313" t="inlineStr">
+        <is>
+          <t>3634.20</t>
+        </is>
+      </c>
+      <c r="AZ313" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="BA313" t="inlineStr">
+        <is>
+          <t>2.77</t>
+        </is>
+      </c>
+      <c r="BB313" t="inlineStr">
+        <is>
+          <t>12871.04</t>
+        </is>
+      </c>
+      <c r="BC313" t="inlineStr">
+        <is>
+          <t>19.0</t>
+        </is>
+      </c>
+      <c r="BD313" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="BE313" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="BF313" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="BG313" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="BH313" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="BI313" t="inlineStr">
+        <is>
+          <t>140649476</t>
         </is>
       </c>
     </row>

</xml_diff>